<commit_message>
New figures, df adjustments
</commit_message>
<xml_diff>
--- a/data/LAPD_Andes_MY.xlsx
+++ b/data/LAPD_Andes_MY.xlsx
@@ -10215,10 +10215,10 @@
         </is>
       </c>
       <c r="H48">
-        <v>-0.333333</v>
+        <v>-0.2</v>
       </c>
       <c r="I48">
-        <v>-79.216667</v>
+        <v>-78.37000000000001</v>
       </c>
       <c r="K48">
         <v>3870</v>

</xml_diff>

<commit_message>
comments added, merged with last R from Ondrej, and cleaned it up a bit. I did not go through all of it.
</commit_message>
<xml_diff>
--- a/data/LAPD_Andes_MY.xlsx
+++ b/data/LAPD_Andes_MY.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Midori\Documents\github\humans-andes\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_scripts\humans-andes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF05DDC-AB1F-46E3-8A54-5628F269C458}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BG$102</definedName>
-  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1456,7 +1452,7 @@
     <t>214; 1242; 213</t>
   </si>
   <si>
-    <t xml:space="preserve">No diagram in PDF_x000D_
+    <t xml:space="preserve">No diagram in PDF_x000D__x000D_
 </t>
   </si>
   <si>
@@ -1478,7 +1474,7 @@
     <t>602</t>
   </si>
   <si>
-    <t xml:space="preserve">Paper is about Cienagra del Visitador_x000D_
+    <t xml:space="preserve">Paper is about Cienagra del Visitador_x000D__x000D_
 </t>
   </si>
   <si>
@@ -1515,7 +1511,7 @@
     <t>3.25</t>
   </si>
   <si>
-    <t xml:space="preserve">DONE_x000D_
+    <t xml:space="preserve">DONE_x000D__x000D_
 </t>
   </si>
   <si>
@@ -1618,6 +1614,9 @@
     <t>Villota et al ,2015</t>
   </si>
   <si>
+    <t>Huila</t>
+  </si>
+  <si>
     <t>Loughlin 2018</t>
   </si>
   <si>
@@ -2189,15 +2188,12 @@
   </si>
   <si>
     <t>843</t>
-  </si>
-  <si>
-    <t>Huila</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2242,7 +2238,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2258,7 +2254,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2333,23 +2329,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2385,23 +2364,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2577,15 +2539,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2766,7 +2730,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2933,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -3100,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -3267,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -3434,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -3595,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -3756,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -3917,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -4078,7 +4042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -4245,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -4412,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -4579,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -4746,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -4907,7 +4871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -5074,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -5235,7 +5199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -5402,7 +5366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -5569,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -5739,7 +5703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -5900,7 +5864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -6067,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -6234,7 +6198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>228</v>
       </c>
@@ -6395,7 +6359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>228</v>
       </c>
@@ -6559,7 +6523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>228</v>
       </c>
@@ -6720,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>228</v>
       </c>
@@ -6881,7 +6845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>228</v>
       </c>
@@ -7048,7 +7012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -7209,7 +7173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -7376,7 +7340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>228</v>
       </c>
@@ -7543,7 +7507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>228</v>
       </c>
@@ -7704,7 +7668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>228</v>
       </c>
@@ -7871,7 +7835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>228</v>
       </c>
@@ -8029,7 +7993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>228</v>
       </c>
@@ -8199,7 +8163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>228</v>
       </c>
@@ -8369,7 +8333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>299</v>
       </c>
@@ -8536,7 +8500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -8706,7 +8670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -8867,7 +8831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -9034,7 +8998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -9195,7 +9159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -9356,7 +9320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -9523,7 +9487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -9690,7 +9654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -9851,7 +9815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -10018,7 +9982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -10179,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -10340,7 +10304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -10501,7 +10465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -10662,7 +10626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -10829,7 +10793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -10996,7 +10960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -11163,7 +11127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -11330,7 +11294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -11491,7 +11455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -11652,7 +11616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -11816,7 +11780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -11977,7 +11941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -12138,7 +12102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -12305,7 +12269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -12472,7 +12436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -12639,7 +12603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -12809,7 +12773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -12979,7 +12943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>477</v>
       </c>
@@ -13146,7 +13110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>484</v>
       </c>
@@ -13307,7 +13271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>491</v>
       </c>
@@ -13474,7 +13438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>496</v>
       </c>
@@ -13641,7 +13605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -13808,7 +13772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -13975,7 +13939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -14115,7 +14079,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="71" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>496</v>
       </c>
@@ -14255,7 +14219,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>496</v>
       </c>
@@ -14403,7 +14367,7 @@
         <v>516</v>
       </c>
       <c r="E73" t="s">
-        <v>721</v>
+        <v>530</v>
       </c>
       <c r="G73" t="s">
         <v>64</v>
@@ -14418,10 +14382,10 @@
         <v>2608</v>
       </c>
       <c r="AX73" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
-    <row r="74" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -14429,16 +14393,16 @@
         <v>1767</v>
       </c>
       <c r="C74" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D74" t="s">
         <v>81</v>
       </c>
       <c r="E74" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F74" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G74" t="s">
         <v>154</v>
@@ -14456,7 +14420,7 @@
         <v>65</v>
       </c>
       <c r="M74" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N74" t="s">
         <v>67</v>
@@ -14588,7 +14552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -14596,16 +14560,16 @@
         <v>958</v>
       </c>
       <c r="C75" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D75" t="s">
         <v>81</v>
       </c>
       <c r="E75" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F75" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="G75" t="s">
         <v>154</v>
@@ -14623,7 +14587,7 @@
         <v>65</v>
       </c>
       <c r="M75" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="N75" t="s">
         <v>67</v>
@@ -14722,7 +14686,7 @@
         <v>75</v>
       </c>
       <c r="AT75" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AV75">
         <v>1980</v>
@@ -14731,13 +14695,13 @@
         <v>1983</v>
       </c>
       <c r="AX75" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="AY75" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="AZ75" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="BA75" t="s">
         <v>276</v>
@@ -14758,24 +14722,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B76">
         <v>1158</v>
       </c>
       <c r="C76" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D76" t="s">
         <v>61</v>
       </c>
       <c r="E76" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F76" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="G76" t="s">
         <v>64</v>
@@ -14793,13 +14757,13 @@
         <v>65</v>
       </c>
       <c r="M76" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="N76" t="s">
         <v>67</v>
       </c>
       <c r="O76" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="P76">
         <v>1</v>
@@ -14898,13 +14862,13 @@
         <v>1999</v>
       </c>
       <c r="AX76" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="AY76" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="AZ76" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="BA76" t="s">
         <v>89</v>
@@ -14925,24 +14889,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B77">
         <v>1184</v>
       </c>
       <c r="C77" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D77" t="s">
         <v>81</v>
       </c>
       <c r="E77" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F77" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="G77" t="s">
         <v>64</v>
@@ -14960,13 +14924,13 @@
         <v>65</v>
       </c>
       <c r="M77" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="N77" t="s">
         <v>67</v>
       </c>
       <c r="O77" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P77">
         <v>1</v>
@@ -15092,24 +15056,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B78">
         <v>1750</v>
       </c>
       <c r="C78" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D78" t="s">
         <v>81</v>
       </c>
       <c r="E78" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F78" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="G78" t="s">
         <v>64</v>
@@ -15127,7 +15091,7 @@
         <v>65</v>
       </c>
       <c r="M78" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N78" t="s">
         <v>67</v>
@@ -15259,24 +15223,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B79">
         <v>1247</v>
       </c>
       <c r="C79" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D79" t="s">
         <v>61</v>
       </c>
       <c r="E79" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F79" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="G79" t="s">
         <v>105</v>
@@ -15294,7 +15258,7 @@
         <v>65</v>
       </c>
       <c r="M79" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="N79" t="s">
         <v>67</v>
@@ -15312,7 +15276,7 @@
         <v>125</v>
       </c>
       <c r="S79" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="T79" t="s">
         <v>70</v>
@@ -15399,13 +15363,13 @@
         <v>2009</v>
       </c>
       <c r="AX79" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="AY79" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="AZ79" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="BA79" t="s">
         <v>89</v>
@@ -15426,24 +15390,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B80">
         <v>1619</v>
       </c>
       <c r="C80" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D80" t="s">
         <v>81</v>
       </c>
       <c r="E80" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F80" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="G80" t="s">
         <v>105</v>
@@ -15461,7 +15425,7 @@
         <v>65</v>
       </c>
       <c r="M80" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="N80" t="s">
         <v>67</v>
@@ -15593,24 +15557,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B81">
         <v>1657</v>
       </c>
       <c r="C81" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D81" t="s">
         <v>81</v>
       </c>
       <c r="E81" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F81" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="G81" t="s">
         <v>105</v>
@@ -15628,7 +15592,7 @@
         <v>65</v>
       </c>
       <c r="M81" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="N81" t="s">
         <v>67</v>
@@ -15643,7 +15607,7 @@
         <v>1</v>
       </c>
       <c r="R81" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="S81" t="s">
         <v>139</v>
@@ -15760,21 +15724,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B82">
         <v>3026</v>
       </c>
       <c r="C82" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D82" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E82" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="G82" t="s">
         <v>105</v>
@@ -15792,7 +15756,7 @@
         <v>65</v>
       </c>
       <c r="M82" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="N82" t="s">
         <v>67</v>
@@ -15810,7 +15774,7 @@
         <v>148</v>
       </c>
       <c r="S82" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="W82">
         <v>2</v>
@@ -15879,7 +15843,7 @@
         <v>2070</v>
       </c>
       <c r="AS82" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="AV82">
         <v>2010</v>
@@ -15888,36 +15852,36 @@
         <v>2016</v>
       </c>
       <c r="AX82" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="AY82" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="AZ82" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="BA82" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B83">
         <v>1615</v>
       </c>
       <c r="C83" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D83" t="s">
         <v>81</v>
       </c>
       <c r="E83" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="F83" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="G83" t="s">
         <v>105</v>
@@ -15935,7 +15899,7 @@
         <v>65</v>
       </c>
       <c r="M83" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="N83" t="s">
         <v>67</v>
@@ -16067,27 +16031,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B84">
         <v>1516</v>
       </c>
       <c r="C84" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D84" t="s">
         <v>81</v>
       </c>
       <c r="E84" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="F84" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="G84" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H84">
         <v>-13.607222</v>
@@ -16102,13 +16066,13 @@
         <v>65</v>
       </c>
       <c r="M84" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="N84" t="s">
         <v>67</v>
       </c>
       <c r="O84" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="P84">
         <v>1</v>
@@ -16195,7 +16159,7 @@
         <v>75</v>
       </c>
       <c r="AT84" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="AV84">
         <v>2000</v>
@@ -16204,13 +16168,13 @@
         <v>2009</v>
       </c>
       <c r="AX84" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="AY84" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="AZ84" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="BA84" t="s">
         <v>89</v>
@@ -16231,27 +16195,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B85">
         <v>1507</v>
       </c>
       <c r="C85" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D85" t="s">
         <v>81</v>
       </c>
       <c r="E85" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="F85" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="G85" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H85">
         <v>-7.3</v>
@@ -16266,13 +16230,13 @@
         <v>65</v>
       </c>
       <c r="M85" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="N85" t="s">
         <v>67</v>
       </c>
       <c r="O85" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="P85">
         <v>0</v>
@@ -16365,7 +16329,7 @@
         <v>75</v>
       </c>
       <c r="AT85" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="AV85">
         <v>2000</v>
@@ -16374,13 +16338,13 @@
         <v>2004</v>
       </c>
       <c r="AX85" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="AY85" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="AZ85" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="BA85" t="s">
         <v>89</v>
@@ -16401,27 +16365,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B86">
         <v>1505</v>
       </c>
       <c r="C86" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D86" t="s">
         <v>81</v>
       </c>
       <c r="E86" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="F86" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G86" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H86">
         <v>-11.783333000000001</v>
@@ -16436,13 +16400,13 @@
         <v>65</v>
       </c>
       <c r="M86" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="N86" t="s">
         <v>67</v>
       </c>
       <c r="O86" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P86">
         <v>1</v>
@@ -16454,13 +16418,13 @@
         <v>69</v>
       </c>
       <c r="S86" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T86" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="U86" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V86" t="s">
         <v>73</v>
@@ -16541,13 +16505,13 @@
         <v>1994</v>
       </c>
       <c r="AX86" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="AY86" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="AZ86" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="BA86" t="s">
         <v>89</v>
@@ -16568,27 +16532,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B87">
         <v>1512</v>
       </c>
       <c r="C87" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D87" t="s">
         <v>81</v>
       </c>
       <c r="E87" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F87" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="G87" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H87">
         <v>-11.666667</v>
@@ -16609,7 +16573,7 @@
         <v>67</v>
       </c>
       <c r="O87" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P87">
         <v>1</v>
@@ -16621,13 +16585,13 @@
         <v>69</v>
       </c>
       <c r="S87" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T87" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="U87" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V87" t="s">
         <v>73</v>
@@ -16708,13 +16672,13 @@
         <v>1994</v>
       </c>
       <c r="AX87" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="AY87" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="AZ87" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="BA87" t="s">
         <v>89</v>
@@ -16735,27 +16699,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B88">
         <v>1506</v>
       </c>
       <c r="C88" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D88" t="s">
         <v>81</v>
       </c>
       <c r="E88" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F88" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="G88" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H88">
         <v>-11</v>
@@ -16770,7 +16734,7 @@
         <v>65</v>
       </c>
       <c r="M88" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="N88" t="s">
         <v>67</v>
@@ -16788,10 +16752,10 @@
         <v>69</v>
       </c>
       <c r="S88" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="U88" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="W88">
         <v>5</v>
@@ -16869,13 +16833,13 @@
         <v>1984</v>
       </c>
       <c r="AX88" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="AY88" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AZ88" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="BA88" t="s">
         <v>89</v>
@@ -16896,27 +16860,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B89">
         <v>1502</v>
       </c>
       <c r="C89" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D89" t="s">
         <v>81</v>
       </c>
       <c r="E89" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F89" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="G89" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H89">
         <v>-7.7</v>
@@ -16931,7 +16895,7 @@
         <v>65</v>
       </c>
       <c r="M89" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="N89" t="s">
         <v>67</v>
@@ -17036,13 +17000,13 @@
         <v>1995</v>
       </c>
       <c r="AX89" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="AY89" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="AZ89" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="BA89" t="s">
         <v>89</v>
@@ -17063,27 +17027,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B90">
         <v>1510</v>
       </c>
       <c r="C90" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D90" t="s">
         <v>81</v>
       </c>
       <c r="E90" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F90" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="G90" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H90">
         <v>-11.783333000000001</v>
@@ -17104,7 +17068,7 @@
         <v>67</v>
       </c>
       <c r="O90" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P90">
         <v>1</v>
@@ -17116,13 +17080,13 @@
         <v>69</v>
       </c>
       <c r="S90" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T90" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="U90" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V90" t="s">
         <v>73</v>
@@ -17203,13 +17167,13 @@
         <v>1994</v>
       </c>
       <c r="AX90" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="AY90" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="AZ90" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="BA90" t="s">
         <v>89</v>
@@ -17230,27 +17194,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B91">
         <v>1513</v>
       </c>
       <c r="C91" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D91" t="s">
         <v>121</v>
       </c>
       <c r="E91" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F91" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G91" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H91">
         <v>-13.951617000000001</v>
@@ -17265,13 +17229,13 @@
         <v>65</v>
       </c>
       <c r="M91" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="N91" t="s">
         <v>67</v>
       </c>
       <c r="O91" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="P91">
         <v>1</v>
@@ -17283,7 +17247,7 @@
         <v>69</v>
       </c>
       <c r="S91" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="U91" t="s">
         <v>372</v>
@@ -17358,7 +17322,7 @@
         <v>75</v>
       </c>
       <c r="AT91" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="AV91">
         <v>2000</v>
@@ -17367,13 +17331,13 @@
         <v>2004</v>
       </c>
       <c r="AX91" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="AY91" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="AZ91" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="BA91" t="s">
         <v>89</v>
@@ -17394,27 +17358,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B92">
         <v>2518</v>
       </c>
       <c r="C92" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D92" t="s">
         <v>81</v>
       </c>
       <c r="E92" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="F92" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="G92" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H92">
         <v>-14.166667</v>
@@ -17429,13 +17393,13 @@
         <v>65</v>
       </c>
       <c r="M92" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="N92" t="s">
         <v>67</v>
       </c>
       <c r="O92" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="P92">
         <v>1</v>
@@ -17444,13 +17408,13 @@
         <v>0</v>
       </c>
       <c r="R92" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="S92" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="T92" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="W92">
         <v>50</v>
@@ -17528,13 +17492,13 @@
         <v>2014</v>
       </c>
       <c r="AX92" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="AY92" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="AZ92" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="BA92" t="s">
         <v>89</v>
@@ -17555,27 +17519,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B93">
         <v>1511</v>
       </c>
       <c r="C93" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D93" t="s">
         <v>81</v>
       </c>
       <c r="E93" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F93" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="G93" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H93">
         <v>-16.399999999999999</v>
@@ -17590,7 +17554,7 @@
         <v>65</v>
       </c>
       <c r="M93" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="N93" t="s">
         <v>67</v>
@@ -17608,16 +17572,16 @@
         <v>69</v>
       </c>
       <c r="S93" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T93" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="U93" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V93" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="W93">
         <v>4</v>
@@ -17689,7 +17653,7 @@
         <v>75</v>
       </c>
       <c r="AT93" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="AV93">
         <v>1990</v>
@@ -17698,13 +17662,13 @@
         <v>1997</v>
       </c>
       <c r="AX93" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="AY93" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="AZ93" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="BA93" t="s">
         <v>89</v>
@@ -17725,27 +17689,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B94">
         <v>1514</v>
       </c>
       <c r="C94" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D94" t="s">
         <v>81</v>
       </c>
       <c r="E94" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F94" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="G94" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H94">
         <v>-13.950278000000001</v>
@@ -17760,7 +17724,7 @@
         <v>65</v>
       </c>
       <c r="M94" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="N94" t="s">
         <v>67</v>
@@ -17778,7 +17742,7 @@
         <v>69</v>
       </c>
       <c r="S94" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="U94" t="s">
         <v>372</v>
@@ -17859,13 +17823,13 @@
         <v>2010</v>
       </c>
       <c r="AX94" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="AY94" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="AZ94" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="BA94" t="s">
         <v>89</v>
@@ -17886,27 +17850,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B95">
         <v>1503</v>
       </c>
       <c r="C95" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D95" t="s">
         <v>121</v>
       </c>
       <c r="E95" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="F95" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="G95" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H95">
         <v>-7.6819439999999997</v>
@@ -17921,7 +17885,7 @@
         <v>65</v>
       </c>
       <c r="M95" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="N95" t="s">
         <v>67</v>
@@ -17939,10 +17903,10 @@
         <v>69</v>
       </c>
       <c r="S95" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="T95" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="U95" t="s">
         <v>73</v>
@@ -18026,13 +17990,13 @@
         <v>2005</v>
       </c>
       <c r="AX95" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="AY95" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="AZ95" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="BA95" t="s">
         <v>89</v>
@@ -18053,27 +18017,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B96">
         <v>1520</v>
       </c>
       <c r="C96" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D96" t="s">
         <v>81</v>
       </c>
       <c r="E96" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="F96" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="G96" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H96">
         <v>-11.390597</v>
@@ -18193,13 +18157,13 @@
         <v>1998</v>
       </c>
       <c r="AX96" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="AY96" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="AZ96" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="BA96" t="s">
         <v>89</v>
@@ -18220,27 +18184,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B97">
         <v>1504</v>
       </c>
       <c r="C97" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="D97" t="s">
         <v>81</v>
       </c>
       <c r="E97" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="F97" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="G97" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H97">
         <v>-10.766667</v>
@@ -18255,7 +18219,7 @@
         <v>65</v>
       </c>
       <c r="M97" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="N97" t="s">
         <v>67</v>
@@ -18273,13 +18237,13 @@
         <v>69</v>
       </c>
       <c r="S97" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T97" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="U97" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V97" t="s">
         <v>73</v>
@@ -18360,16 +18324,16 @@
         <v>1984</v>
       </c>
       <c r="AX97" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="AY97" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="AZ97" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="BA97" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="BB97">
         <v>2983.333333</v>
@@ -18387,27 +18351,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B98">
         <v>1546</v>
       </c>
       <c r="C98" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D98" t="s">
         <v>121</v>
       </c>
       <c r="E98" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="F98" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="G98" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H98">
         <v>-15.5</v>
@@ -18422,7 +18386,7 @@
         <v>65</v>
       </c>
       <c r="M98" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="N98" t="s">
         <v>67</v>
@@ -18440,13 +18404,13 @@
         <v>125</v>
       </c>
       <c r="S98" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T98" t="s">
         <v>71</v>
       </c>
       <c r="U98" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V98" t="s">
         <v>73</v>
@@ -18527,13 +18491,13 @@
         <v>2012</v>
       </c>
       <c r="AX98" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="AY98" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="AZ98" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="BA98" t="s">
         <v>89</v>
@@ -18554,27 +18518,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B99">
         <v>1496</v>
       </c>
       <c r="C99" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="D99" t="s">
         <v>81</v>
       </c>
       <c r="E99" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="F99" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="G99" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H99">
         <v>-14.183332999999999</v>
@@ -18589,13 +18553,13 @@
         <v>65</v>
       </c>
       <c r="M99" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="N99" t="s">
         <v>67</v>
       </c>
       <c r="O99" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="P99">
         <v>1</v>
@@ -18607,13 +18571,13 @@
         <v>86</v>
       </c>
       <c r="S99" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T99" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="U99" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V99" t="s">
         <v>72</v>
@@ -18694,13 +18658,13 @@
         <v>2007</v>
       </c>
       <c r="AX99" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="AY99" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="AZ99" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="BA99" t="s">
         <v>89</v>
@@ -18721,24 +18685,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B100">
         <v>1715</v>
       </c>
       <c r="C100" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D100" t="s">
         <v>81</v>
       </c>
       <c r="E100" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="F100" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="G100" t="s">
         <v>154</v>
@@ -18762,7 +18726,7 @@
         <v>67</v>
       </c>
       <c r="O100" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="P100">
         <v>1</v>
@@ -18771,7 +18735,7 @@
         <v>0</v>
       </c>
       <c r="R100" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="S100" t="s">
         <v>71</v>
@@ -18855,13 +18819,13 @@
         <v>1978</v>
       </c>
       <c r="AX100" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="AY100" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AZ100" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="BA100" t="s">
         <v>89</v>
@@ -18882,24 +18846,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B101">
         <v>1744</v>
       </c>
       <c r="C101" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D101" t="s">
         <v>81</v>
       </c>
       <c r="E101" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="F101" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="G101" t="s">
         <v>64</v>
@@ -18917,7 +18881,7 @@
         <v>65</v>
       </c>
       <c r="M101" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="N101" t="s">
         <v>67</v>
@@ -19043,24 +19007,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:58" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B102">
         <v>1157</v>
       </c>
       <c r="C102" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D102" t="s">
         <v>81</v>
       </c>
       <c r="E102" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F102" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="G102" t="s">
         <v>64</v>
@@ -19078,13 +19042,13 @@
         <v>65</v>
       </c>
       <c r="M102" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="N102" t="s">
         <v>67</v>
       </c>
       <c r="O102" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="P102">
         <v>1</v>
@@ -19183,13 +19147,13 @@
         <v>2010</v>
       </c>
       <c r="AX102" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="AY102" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="AZ102" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="BA102" t="s">
         <v>89</v>
@@ -19211,13 +19175,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BG102" xr:uid="{4890A21C-0194-4651-A054-367B04F2BBDF}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Huila_x000d__x000a_"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>